<commit_message>
Update MagIC Excel Template
</commit_message>
<xml_diff>
--- a/.public/MagIC/Template3.0ForMagICUpload.xlsx
+++ b/.public/MagIC/Template3.0ForMagICUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10307"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njarboe/Dropbox/MagIC/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D89E3237-3E12-604B-88A7-8620658062E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C238F40-9955-BD45-B1B0-EE9D8F422C43}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18720" yWindow="3640" windowWidth="30400" windowHeight="17180" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21500" yWindow="8140" windowWidth="28800" windowHeight="17000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="locations" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="94">
   <si>
     <t>location</t>
   </si>
@@ -160,9 +160,6 @@
     <t>dir_n_total_samples</t>
   </si>
   <si>
-    <t>Required: at least one of location, site, sample, specimen</t>
-  </si>
-  <si>
     <t>Please include a method code that describes the dating method</t>
   </si>
   <si>
@@ -314,13 +311,19 @@
   </si>
   <si>
     <t>Bay of Bengal</t>
+  </si>
+  <si>
+    <t>This table is used for ages determined in the paper associated with the paper</t>
+  </si>
+  <si>
+    <t>external_database_ids</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -400,6 +403,21 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -418,14 +436,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -437,12 +456,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="5" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -723,8 +745,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S18" sqref="S18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -740,32 +762,32 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O1" t="s">
+        <v>88</v>
+      </c>
+      <c r="P1" t="s">
         <v>89</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>91</v>
-      </c>
-      <c r="R1" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -792,25 +814,25 @@
       <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="O2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="P2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="4" t="s">
+      <c r="Q2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="12" t="s">
         <v>16</v>
       </c>
       <c r="T2" s="7" t="s">
@@ -818,6 +840,17 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{9C34F620-28DD-584C-81E7-7005AEAE7241}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{446F0401-45C5-6A45-86FC-B28AF52A05B1}"/>
+    <hyperlink ref="D2" r:id="rId3" xr:uid="{E96087E6-3612-CB44-9987-3C7711184554}"/>
+    <hyperlink ref="O2" r:id="rId4" xr:uid="{23D353E8-954C-544B-A7BB-B9C72C378727}"/>
+    <hyperlink ref="P2" r:id="rId5" xr:uid="{67A62DCE-2283-234B-AD9C-E102A35B29CE}"/>
+    <hyperlink ref="Q2" r:id="rId6" xr:uid="{CCEF7671-6222-114A-9977-FCF80F12A0F2}"/>
+    <hyperlink ref="R2" r:id="rId7" xr:uid="{4FAFED3C-50B5-5048-BF14-1B5F7B457148}"/>
+    <hyperlink ref="S2" r:id="rId8" xr:uid="{93B82F0D-35CE-404F-8AA8-454E6308443F}"/>
+    <hyperlink ref="M2" r:id="rId9" xr:uid="{2674D4CC-35D4-1847-B325-D51AC3116BD8}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -828,7 +861,7 @@
   <dimension ref="A1:Z2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -846,7 +879,7 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:26" ht="17" x14ac:dyDescent="0.2">
@@ -856,16 +889,16 @@
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -886,7 +919,7 @@
       <c r="L2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="11" t="s">
         <v>12</v>
       </c>
       <c r="N2" s="2" t="s">
@@ -920,16 +953,23 @@
         <v>38</v>
       </c>
       <c r="X2" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="Y2" s="6" t="s">
-        <v>46</v>
-      </c>
       <c r="Z2" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{E806FDCE-A996-9740-992F-ADA9B1F4CC28}"/>
+    <hyperlink ref="F2" r:id="rId2" xr:uid="{946ECC33-6397-0F4E-A9DF-4370EA562670}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{56583B7E-F643-2745-BD6D-74D3AC45133F}"/>
+    <hyperlink ref="C2" r:id="rId4" xr:uid="{A1ACE978-A1A9-7247-97B3-79C6EE3E96CF}"/>
+    <hyperlink ref="M2" r:id="rId5" xr:uid="{D4B2482E-89C5-7B41-8349-F7A1F0AC2D43}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -940,7 +980,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1048576"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -950,12 +990,12 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -965,7 +1005,7 @@
       <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -981,10 +1021,13 @@
         <v>20</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{DAFE0553-C6F4-7640-BB8C-254BE913163E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -994,7 +1037,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1005,7 +1048,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -1015,7 +1058,7 @@
       <c r="B2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -1037,13 +1080,16 @@
         <v>34</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>46</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{7A2EDDE2-F721-764A-B4FC-A7FF1A78C260}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1052,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1074,66 +1120,66 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
         <v>59</v>
       </c>
-      <c r="K1" t="s">
-        <v>60</v>
-      </c>
       <c r="M1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W1" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" t="s">
         <v>69</v>
-      </c>
-      <c r="X1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s">
         <v>83</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>84</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" t="s">
         <v>85</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>86</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>87</v>
-      </c>
-      <c r="M2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="17" x14ac:dyDescent="0.2">
@@ -1147,7 +1193,7 @@
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>28</v>
@@ -1155,7 +1201,7 @@
       <c r="F3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="11" t="s">
         <v>16</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -1165,37 +1211,37 @@
         <v>30</v>
       </c>
       <c r="J3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="L3" s="5" t="s">
+      <c r="M3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="N3" s="5" t="s">
-        <v>57</v>
-      </c>
       <c r="O3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="P3" s="5" t="s">
+      <c r="Q3" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="R3" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="Q3" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="R3" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="S3" s="5" t="s">
-        <v>64</v>
-      </c>
       <c r="T3" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U3" s="5" t="s">
         <v>33</v>
@@ -1204,13 +1250,16 @@
         <v>34</v>
       </c>
       <c r="W3" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="X3" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="X3" s="5" t="s">
-        <v>68</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G3" r:id="rId1" xr:uid="{D9599BEB-D39E-E94A-A11B-EECB49B8CECA}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1219,7 +1268,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1230,60 +1281,64 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="E2" s="9" t="s">
         <v>17</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A6D71CDD-3B29-6946-82EA-0BEAB50A3F4D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="16" customWidth="1"/>
-    <col min="9" max="9" width="39.1640625" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="13.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" t="s">
         <v>41</v>
       </c>
-      <c r="E1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1311,14 +1366,20 @@
       <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="J2" s="11" t="s">
         <v>16</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="L2" s="9" t="s">
+        <v>93</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{FEDEE117-2269-304D-B46F-F57EDE9FE2DD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1328,7 +1389,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1338,27 +1399,27 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>81</v>
-      </c>
       <c r="F2" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>